<commit_message>
Snippet filler support output a list joint by a split string while filling instance info.
</commit_message>
<xml_diff>
--- a/dat/DEMO_ES/conf.xlsx
+++ b/dat/DEMO_ES/conf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18352" windowHeight="8265" activeTab="2"/>
+    <workbookView windowWidth="18352" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="HOSTS" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="METRICS" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSTS!$A$2:$N$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSTS!$A$2:$O$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <t>ssh</t>
   </si>
@@ -47,6 +47,9 @@
     <t>ES</t>
   </si>
   <si>
+    <t>Kibana</t>
+  </si>
+  <si>
     <t>序号</t>
   </si>
   <si>
@@ -65,49 +68,49 @@
     <t>master</t>
   </si>
   <si>
+    <t>data_content</t>
+  </si>
+  <si>
+    <t>data_hot</t>
+  </si>
+  <si>
+    <t>data_warm</t>
+  </si>
+  <si>
+    <t>data_cold</t>
+  </si>
+  <si>
+    <t>transport</t>
+  </si>
+  <si>
+    <t>httport</t>
+  </si>
+  <si>
+    <t>192.168.1.1</t>
+  </si>
+  <si>
+    <t>demo-192-168-1-1</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>data</t>
   </si>
   <si>
-    <t>coord</t>
-  </si>
-  <si>
     <t>kibana</t>
   </si>
   <si>
-    <t>transport</t>
-  </si>
-  <si>
-    <t>httport</t>
-  </si>
-  <si>
-    <t>192.168.1.1</t>
-  </si>
-  <si>
-    <t>demo-192-168-1-1</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>hot</t>
-  </si>
-  <si>
     <t>192.168.1.2</t>
   </si>
   <si>
     <t>demo-192-168-1-2</t>
   </si>
   <si>
-    <t>warm</t>
-  </si>
-  <si>
     <t>192.168.1.3</t>
   </si>
   <si>
     <t>demo-192-168-1-3</t>
-  </si>
-  <si>
-    <t>cold</t>
   </si>
   <si>
     <t>java_home</t>
@@ -1231,14 +1234,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1251,10 +1254,10 @@
     <col min="6" max="6" width="4.87610619469027" customWidth="1"/>
     <col min="7" max="7" width="7.50442477876106" customWidth="1"/>
     <col min="8" max="8" width="7.75221238938053" customWidth="1"/>
-    <col min="9" max="14" width="8.6283185840708" customWidth="1"/>
+    <col min="9" max="15" width="8.6283185840708" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1277,103 +1280,113 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="7"/>
+      <c r="P1" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>15</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="10"/>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="9" t="str">
         <f>D3&amp;"-"&amp;C3&amp;"-"&amp;H3</f>
         <v>master-demo-192-168-1-1-1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7">
         <v>1</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
-      <c r="M3" s="7" t="str">
+      <c r="M3" s="7"/>
+      <c r="N3" s="7" t="str">
         <f>"930"&amp;H3</f>
         <v>9301</v>
       </c>
-      <c r="N3" s="7" t="str">
+      <c r="O3" s="7" t="str">
         <f>"920"&amp;H3</f>
         <v>9201</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E4" s="9" t="str">
-        <f t="shared" ref="E4:E10" si="0">D4&amp;"-"&amp;C4&amp;"-"&amp;H4</f>
+        <f>D4&amp;"-"&amp;C4&amp;"-"&amp;H4</f>
         <v>data-demo-192-168-1-1-2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7">
@@ -1381,38 +1394,42 @@
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="L4" s="7"/>
-      <c r="M4" s="7" t="str">
-        <f t="shared" ref="M4:M10" si="1">"930"&amp;H4</f>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7" t="str">
+        <f>"930"&amp;H4</f>
         <v>9302</v>
       </c>
-      <c r="N4" s="7" t="str">
-        <f t="shared" ref="N4:N10" si="2">"920"&amp;H4</f>
+      <c r="O4" s="7" t="str">
+        <f>"920"&amp;H4</f>
         <v>9202</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="9">
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E5" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>D5&amp;"-"&amp;C5&amp;"-"&amp;H5</f>
         <v>kibana-demo-192-168-1-1-3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7">
@@ -1421,76 +1438,80 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7" t="str">
+        <f>"930"&amp;H5</f>
         <v>9303</v>
       </c>
-      <c r="N5" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="O5" s="7" t="str">
+        <f>"920"&amp;H5</f>
         <v>9203</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="P5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="9" t="str">
+        <f>D6&amp;"-"&amp;C6&amp;"-"&amp;H6</f>
+        <v>master-demo-192-168-1-2-1</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>master-demo-192-168-1-2-1</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7">
         <v>1</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7" t="str">
+        <f>"930"&amp;H6</f>
         <v>9301</v>
       </c>
-      <c r="N6" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="O6" s="7" t="str">
+        <f>"920"&amp;H6</f>
         <v>9201</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="9">
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="9" t="str">
+        <f>D7&amp;"-"&amp;C7&amp;"-"&amp;H7</f>
+        <v>data-demo-192-168-1-2-2</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>data-demo-192-168-1-2-2</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7">
@@ -1498,146 +1519,118 @@
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7" t="str">
-        <f t="shared" si="1"/>
+      <c r="L7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7" t="str">
+        <f>"930"&amp;H7</f>
         <v>9302</v>
       </c>
-      <c r="N7" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="O7" s="7" t="str">
+        <f>"920"&amp;H7</f>
         <v>9202</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:16">
       <c r="A8" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="9" t="str">
+        <f>D8&amp;"-"&amp;C8&amp;"-"&amp;H8</f>
+        <v>master-demo-192-168-1-3-1</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>coord-demo-192-168-1-2-3</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7">
-        <v>3</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7" t="s">
-        <v>17</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>9303</v>
-      </c>
+      <c r="M8" s="7"/>
       <c r="N8" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>9203</v>
-      </c>
-    </row>
-    <row r="9" customHeight="1" spans="1:14">
+        <f>"930"&amp;H8</f>
+        <v>9301</v>
+      </c>
+      <c r="O8" s="7" t="str">
+        <f>"920"&amp;H8</f>
+        <v>9201</v>
+      </c>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" customFormat="1" customHeight="1" spans="1:16">
       <c r="A9" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>master-demo-192-168-1-3-1</v>
+        <f>D9&amp;"-"&amp;C9&amp;"-"&amp;H9</f>
+        <v>data-demo-192-168-1-3-2</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7">
-        <v>1</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>17</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>9301</v>
+      <c r="M9" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="N9" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>9201</v>
-      </c>
-    </row>
-    <row r="10" customFormat="1" customHeight="1" spans="1:14">
-      <c r="A10" s="9">
-        <v>8</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>data-demo-192-168-1-3-2</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7">
-        <v>2</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>"930"&amp;H9</f>
         <v>9302</v>
       </c>
-      <c r="N10" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="O9" s="7" t="str">
+        <f>"920"&amp;H9</f>
         <v>9202</v>
       </c>
+      <c r="P9" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N10">
+  <autoFilter ref="A2:O9">
     <extLst/>
   </autoFilter>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="I1:O1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="P1:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1662,58 +1655,58 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:2">
@@ -1754,7 +1747,7 @@
   <sheetPr/>
   <dimension ref="B1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1797,66 +1790,66 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>